<commit_message>
handle empty row data
</commit_message>
<xml_diff>
--- a/obligations.xlsx
+++ b/obligations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t xml:space="preserve">Description*</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">Error (missing required)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test empty Desc</t>
   </si>
 </sst>
 </file>
@@ -214,7 +217,7 @@
   <dimension ref="A1:G1005"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -336,7 +339,15 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="7"/>

</xml_diff>

<commit_message>
create a sample, update comments
</commit_message>
<xml_diff>
--- a/obligations.xlsx
+++ b/obligations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">Description*</t>
   </si>
@@ -41,39 +41,6 @@
   </si>
   <si>
     <t xml:space="preserve">Day of Month</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Car</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Loan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Audi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shared</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Credit Card</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Huntington</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Internet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verizon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Groceries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expense</t>
   </si>
 </sst>
 </file>
@@ -208,10 +175,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1003"/>
+  <dimension ref="A1:G995"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -250,78 +217,22 @@
       </c>
     </row>
     <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>10000</v>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>292.58</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>9</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>3000</v>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>135</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>12</v>
-      </c>
+      <c r="B3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>99</v>
-      </c>
-      <c r="G4" s="1" t="n">
-        <v>17</v>
-      </c>
+      <c r="B4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>1000</v>
-      </c>
+      <c r="B5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="7"/>
@@ -3293,33 +3204,9 @@
     <row r="995" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B995" s="7"/>
     </row>
-    <row r="996" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B996" s="7"/>
-    </row>
-    <row r="997" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B997" s="7"/>
-    </row>
-    <row r="998" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B998" s="7"/>
-    </row>
-    <row r="999" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B999" s="7"/>
-    </row>
-    <row r="1000" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1000" s="7"/>
-    </row>
-    <row r="1001" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1001" s="7"/>
-    </row>
-    <row r="1002" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1002" s="7"/>
-    </row>
-    <row r="1003" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1003" s="7"/>
-    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B1003" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B995" type="list">
       <formula1>"Loan,Credit Card,Bill,Expense"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>